<commit_message>
Budget Update Sept 07
</commit_message>
<xml_diff>
--- a/source files/budget_jeanre.xlsx
+++ b/source files/budget_jeanre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/GIT Repos/ftrack/source files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FC03C3-ECA3-114F-9F2B-218036F933C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EFF33D-2BA1-7347-B6B7-3954C5F13473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="18700" activeTab="5" xr2:uid="{F25DD163-696E-F842-A897-5E899A2812A7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{F25DD163-696E-F842-A897-5E899A2812A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Jeanre Transactional" sheetId="11" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="90">
   <si>
     <t>Jeanre Transactional</t>
   </si>
@@ -305,6 +305,15 @@
   <si>
     <t>Bernice Personal Savings</t>
   </si>
+  <si>
+    <t>Tax Refund</t>
+  </si>
+  <si>
+    <t>Vape</t>
+  </si>
+  <si>
+    <t>Gaming</t>
+  </si>
 </sst>
 </file>
 
@@ -313,7 +322,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -444,6 +453,13 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -617,7 +633,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -677,827 +693,13 @@
     <xf numFmtId="44" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="18" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="222">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2367,6 +1569,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2391,6 +1617,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2415,6 +1665,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2439,6 +1713,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2463,6 +1761,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2487,6 +1809,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2511,6 +1857,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2535,6 +1905,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2559,6 +1953,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2583,6 +2001,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2607,6 +2049,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2631,6 +2097,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2655,6 +2145,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2679,6 +2193,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2703,6 +2241,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2727,6 +2289,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2751,6 +2337,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2775,6 +2385,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2799,6 +2433,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2823,6 +2481,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2847,6 +2529,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2871,6 +2577,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2895,6 +2625,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -2919,6 +2673,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
         <scheme val="none"/>
@@ -3125,18 +2903,258 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -5989,33 +6007,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3E63981-326C-D143-B66A-6C003C4E74A8}" name="Table32" displayName="Table32" ref="A1:J30" totalsRowCount="1" headerRowDxfId="221" dataDxfId="220">
-  <autoFilter ref="A1:J29" xr:uid="{92565AF6-51CB-F740-ACD0-AD376C5F8FE0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3E63981-326C-D143-B66A-6C003C4E74A8}" name="Table32" displayName="Table32" ref="A1:J32" totalsRowCount="1" headerRowDxfId="221" dataDxfId="220">
+  <autoFilter ref="A1:J31" xr:uid="{92565AF6-51CB-F740-ACD0-AD376C5F8FE0}"/>
   <tableColumns count="10">
-    <tableColumn id="5" xr3:uid="{8651B483-0F4C-9745-8034-DD83AE8DA141}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="219" totalsRowDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{2F7AE88F-4B40-4240-BF3E-94BC56EB2208}" name="Account Secondary" totalsRowLabel="Jeanre Transactional" dataDxfId="218" totalsRowDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{ADA98953-117B-F145-A74B-A985F167B6BC}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="217" totalsRowDxfId="41">
+    <tableColumn id="5" xr3:uid="{8651B483-0F4C-9745-8034-DD83AE8DA141}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="219" totalsRowDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{2F7AE88F-4B40-4240-BF3E-94BC56EB2208}" name="Account Secondary" totalsRowLabel="Jeanre Transactional" dataDxfId="218" totalsRowDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{ADA98953-117B-F145-A74B-A985F167B6BC}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="217" totalsRowDxfId="7">
       <totalsRowFormula>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-05-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-05-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{D1B507DF-9E64-6B42-ADC6-664BF896B5B8}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="216" totalsRowDxfId="40">
+    <tableColumn id="8" xr3:uid="{D1B507DF-9E64-6B42-ADC6-664BF896B5B8}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="216" totalsRowDxfId="6">
       <totalsRowFormula>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-06-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-06-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C4FB259E-8339-874F-86A0-1B451C317784}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="215" totalsRowDxfId="39">
+    <tableColumn id="9" xr3:uid="{C4FB259E-8339-874F-86A0-1B451C317784}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="215" totalsRowDxfId="5">
       <totalsRowFormula>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-07-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-07-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{7CAB3A22-E21F-C14F-81D6-E08D7B5AAF27}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="214" totalsRowDxfId="38">
+    <tableColumn id="10" xr3:uid="{7CAB3A22-E21F-C14F-81D6-E08D7B5AAF27}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="214" totalsRowDxfId="4">
       <totalsRowFormula>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-08-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-08-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{A858D8D8-0330-2A48-9F9F-65775EFA0FA2}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="213" totalsRowDxfId="37">
+    <tableColumn id="11" xr3:uid="{A858D8D8-0330-2A48-9F9F-65775EFA0FA2}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="213" totalsRowDxfId="3">
       <totalsRowFormula>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-09-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-09-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{272E93CF-FAFA-2340-9C46-83694C73D7CE}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="212" totalsRowDxfId="36">
+    <tableColumn id="12" xr3:uid="{272E93CF-FAFA-2340-9C46-83694C73D7CE}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="212" totalsRowDxfId="2">
       <totalsRowFormula>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-10-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-10-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{7E46E0A7-4F44-7B4D-A98B-07E6BFFF5704}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="211" totalsRowDxfId="35">
+    <tableColumn id="13" xr3:uid="{7E46E0A7-4F44-7B4D-A98B-07E6BFFF5704}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="211" totalsRowDxfId="1">
       <totalsRowFormula>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-11-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-11-01]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{3415A647-D2D3-BE4C-A006-2DADF61AE0D7}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="210" totalsRowDxfId="34">
+    <tableColumn id="14" xr3:uid="{3415A647-D2D3-BE4C-A006-2DADF61AE0D7}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="210" totalsRowDxfId="0">
       <totalsRowFormula>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-12-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-12-01]])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -6043,8 +6061,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B198D46-04BB-0942-B50C-97F8D19A9484}" name="Table323" displayName="Table323" ref="A1:J5" totalsRowShown="0" headerRowDxfId="197" dataDxfId="196">
-  <autoFilter ref="A1:J5" xr:uid="{92565AF6-51CB-F740-ACD0-AD376C5F8FE0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B198D46-04BB-0942-B50C-97F8D19A9484}" name="Table323" displayName="Table323" ref="A1:J6" totalsRowShown="0" headerRowDxfId="197" dataDxfId="196">
+  <autoFilter ref="A1:J6" xr:uid="{92565AF6-51CB-F740-ACD0-AD376C5F8FE0}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{0B7A1F2D-D042-6947-B65B-356D4D33EC84}" name="Movement" dataDxfId="195"/>
     <tableColumn id="6" xr3:uid="{8D570864-DCAB-384F-9AAB-0B1B408BA72D}" name="Account Secondary" dataDxfId="194"/>
@@ -6191,102 +6209,102 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{21702B49-2777-3448-9DCF-365AAD4235B1}" name="Table328" displayName="Table328" ref="A1:AH8" totalsRowCount="1" headerRowDxfId="103" dataDxfId="102">
   <autoFilter ref="A1:AH7" xr:uid="{92565AF6-51CB-F740-ACD0-AD376C5F8FE0}"/>
   <tableColumns count="34">
-    <tableColumn id="1" xr3:uid="{132F1BF4-3588-8A4B-8F98-DB76AAE601DC}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="101" totalsRowDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{81ACCF9B-B060-EC46-8372-B215BC3E24E6}" name="Account Secondary" totalsRowLabel="Jodine U" dataDxfId="100" totalsRowDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{984BE13D-B3F0-4141-8171-AF453C2EDE3E}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="99" totalsRowDxfId="31">
+    <tableColumn id="1" xr3:uid="{132F1BF4-3588-8A4B-8F98-DB76AAE601DC}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="101" totalsRowDxfId="100"/>
+    <tableColumn id="6" xr3:uid="{81ACCF9B-B060-EC46-8372-B215BC3E24E6}" name="Account Secondary" totalsRowLabel="Jodine U" dataDxfId="99" totalsRowDxfId="98"/>
+    <tableColumn id="7" xr3:uid="{984BE13D-B3F0-4141-8171-AF453C2EDE3E}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="97" totalsRowDxfId="96">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2024-05-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2024-05-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2BB3D3C5-F012-FD47-A358-58BB6A556D7D}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="98" totalsRowDxfId="30">
+    <tableColumn id="8" xr3:uid="{2BB3D3C5-F012-FD47-A358-58BB6A556D7D}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="95" totalsRowDxfId="94">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2024-06-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2024-06-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{EBB6AB3B-A446-DB4F-8264-72B3190C9CED}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="97" totalsRowDxfId="29">
+    <tableColumn id="9" xr3:uid="{EBB6AB3B-A446-DB4F-8264-72B3190C9CED}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="93" totalsRowDxfId="92">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2024-07-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2024-07-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{DBE96D9B-9F27-8F47-86E4-7AAF262DF5C8}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="96" totalsRowDxfId="28">
+    <tableColumn id="10" xr3:uid="{DBE96D9B-9F27-8F47-86E4-7AAF262DF5C8}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="91" totalsRowDxfId="90">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2024-08-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2024-08-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{6462287A-231A-F94A-AFF2-718E314EBE0D}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="95" totalsRowDxfId="27">
+    <tableColumn id="11" xr3:uid="{6462287A-231A-F94A-AFF2-718E314EBE0D}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="89" totalsRowDxfId="88">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2024-09-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2024-09-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{7D2A10AB-97F3-9446-95E7-2824AB9C1D8B}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="94" totalsRowDxfId="26">
+    <tableColumn id="12" xr3:uid="{7D2A10AB-97F3-9446-95E7-2824AB9C1D8B}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="87" totalsRowDxfId="86">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2024-10-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2024-10-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{85B33C4E-94DF-EC4C-8640-5B925E92396A}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="93" totalsRowDxfId="25">
+    <tableColumn id="13" xr3:uid="{85B33C4E-94DF-EC4C-8640-5B925E92396A}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="85" totalsRowDxfId="84">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2024-11-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2024-11-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{54118784-7FBB-8442-9E75-D434EAE0D358}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="92" totalsRowDxfId="24">
+    <tableColumn id="14" xr3:uid="{54118784-7FBB-8442-9E75-D434EAE0D358}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="83" totalsRowDxfId="82">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2024-12-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2024-12-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{11E91D47-A42F-6F4F-8643-BBA17A2766CE}" name="2025-01-01" totalsRowFunction="custom" dataDxfId="91" totalsRowDxfId="23">
+    <tableColumn id="15" xr3:uid="{11E91D47-A42F-6F4F-8643-BBA17A2766CE}" name="2025-01-01" totalsRowFunction="custom" dataDxfId="81" totalsRowDxfId="80">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2025-01-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2025-01-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{A9F69F66-C1FE-A346-BC10-3BD28F4560DC}" name="2025-02-01" totalsRowFunction="custom" dataDxfId="90" totalsRowDxfId="22">
+    <tableColumn id="16" xr3:uid="{A9F69F66-C1FE-A346-BC10-3BD28F4560DC}" name="2025-02-01" totalsRowFunction="custom" dataDxfId="79" totalsRowDxfId="78">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2025-02-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2025-02-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{F4313802-9F49-A249-829D-BE1DAC00470C}" name="2025-03-01" totalsRowFunction="custom" dataDxfId="89" totalsRowDxfId="21">
+    <tableColumn id="17" xr3:uid="{F4313802-9F49-A249-829D-BE1DAC00470C}" name="2025-03-01" totalsRowFunction="custom" dataDxfId="77" totalsRowDxfId="76">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2025-03-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2025-03-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{70DCD78C-734A-2A4F-96D9-75E2F722BBEF}" name="2025-04-01" totalsRowFunction="custom" dataDxfId="88" totalsRowDxfId="20">
+    <tableColumn id="18" xr3:uid="{70DCD78C-734A-2A4F-96D9-75E2F722BBEF}" name="2025-04-01" totalsRowFunction="custom" dataDxfId="75" totalsRowDxfId="74">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2025-04-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2025-04-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{3CB93C70-C607-C849-9D6E-A12F48DB0917}" name="2025-05-01" totalsRowFunction="custom" dataDxfId="87" totalsRowDxfId="19">
+    <tableColumn id="19" xr3:uid="{3CB93C70-C607-C849-9D6E-A12F48DB0917}" name="2025-05-01" totalsRowFunction="custom" dataDxfId="73" totalsRowDxfId="72">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2025-05-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2025-05-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{8B2DFDEA-F50F-564E-88EB-40B3ADE38284}" name="2025-06-01" totalsRowFunction="custom" dataDxfId="86" totalsRowDxfId="18">
+    <tableColumn id="20" xr3:uid="{8B2DFDEA-F50F-564E-88EB-40B3ADE38284}" name="2025-06-01" totalsRowFunction="custom" dataDxfId="71" totalsRowDxfId="70">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2025-06-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2025-06-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{91AB2B18-50E8-D042-B65D-FE4C52807967}" name="2025-07-01" totalsRowFunction="custom" dataDxfId="85" totalsRowDxfId="17">
+    <tableColumn id="21" xr3:uid="{91AB2B18-50E8-D042-B65D-FE4C52807967}" name="2025-07-01" totalsRowFunction="custom" dataDxfId="69" totalsRowDxfId="68">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2025-07-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2025-07-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{1B34BB85-1C48-D24A-AECB-C60DA7FC690D}" name="2025-08-01" totalsRowFunction="custom" dataDxfId="84" totalsRowDxfId="16">
+    <tableColumn id="22" xr3:uid="{1B34BB85-1C48-D24A-AECB-C60DA7FC690D}" name="2025-08-01" totalsRowFunction="custom" dataDxfId="67" totalsRowDxfId="66">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2025-08-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2025-08-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{6AA34C9A-7D16-4045-8E67-CAA0588D1E20}" name="2025-09-01" totalsRowFunction="custom" dataDxfId="83" totalsRowDxfId="15">
+    <tableColumn id="23" xr3:uid="{6AA34C9A-7D16-4045-8E67-CAA0588D1E20}" name="2025-09-01" totalsRowFunction="custom" dataDxfId="65" totalsRowDxfId="64">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2025-09-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2025-09-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{F76057EE-251C-8347-AA7B-C0BD03E23E1B}" name="2025-10-01" totalsRowFunction="custom" dataDxfId="82" totalsRowDxfId="14">
+    <tableColumn id="24" xr3:uid="{F76057EE-251C-8347-AA7B-C0BD03E23E1B}" name="2025-10-01" totalsRowFunction="custom" dataDxfId="63" totalsRowDxfId="62">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2025-10-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2025-10-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{B3CED7D0-5665-8843-BB8D-DD4B2D475330}" name="2025-11-01" totalsRowFunction="custom" dataDxfId="81" totalsRowDxfId="13">
+    <tableColumn id="25" xr3:uid="{B3CED7D0-5665-8843-BB8D-DD4B2D475330}" name="2025-11-01" totalsRowFunction="custom" dataDxfId="61" totalsRowDxfId="60">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2025-11-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2025-11-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{17986AF3-FF29-0945-9531-7F4A42463D68}" name="2025-12-01" totalsRowFunction="custom" dataDxfId="80" totalsRowDxfId="12">
+    <tableColumn id="26" xr3:uid="{17986AF3-FF29-0945-9531-7F4A42463D68}" name="2025-12-01" totalsRowFunction="custom" dataDxfId="59" totalsRowDxfId="58">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2025-12-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2025-12-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{A0E3385D-60FC-124E-ACB2-3CF5068E197E}" name="2026-01-01" totalsRowFunction="custom" dataDxfId="79" totalsRowDxfId="11">
+    <tableColumn id="27" xr3:uid="{A0E3385D-60FC-124E-ACB2-3CF5068E197E}" name="2026-01-01" totalsRowFunction="custom" dataDxfId="57" totalsRowDxfId="56">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2026-01-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2026-01-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{2B18E388-6340-864F-94E0-B6C712B3E140}" name="2026-02-01" totalsRowFunction="custom" dataDxfId="78" totalsRowDxfId="10">
+    <tableColumn id="28" xr3:uid="{2B18E388-6340-864F-94E0-B6C712B3E140}" name="2026-02-01" totalsRowFunction="custom" dataDxfId="55" totalsRowDxfId="54">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2026-02-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2026-02-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{A56D1D1A-BCDD-3A4E-996A-4D01DADFF67B}" name="2026-03-01" totalsRowFunction="custom" dataDxfId="77" totalsRowDxfId="9">
+    <tableColumn id="29" xr3:uid="{A56D1D1A-BCDD-3A4E-996A-4D01DADFF67B}" name="2026-03-01" totalsRowFunction="custom" dataDxfId="53" totalsRowDxfId="52">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2026-03-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2026-03-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{A90A62ED-9074-8848-A318-D26D567C3D87}" name="2026-04-01" totalsRowFunction="custom" dataDxfId="76" totalsRowDxfId="8">
+    <tableColumn id="30" xr3:uid="{A90A62ED-9074-8848-A318-D26D567C3D87}" name="2026-04-01" totalsRowFunction="custom" dataDxfId="51" totalsRowDxfId="50">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2026-04-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2026-04-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{FC125C77-2688-F547-86F6-9B4B045F6EEF}" name="2026-05-01" totalsRowFunction="custom" dataDxfId="75" totalsRowDxfId="7">
+    <tableColumn id="31" xr3:uid="{FC125C77-2688-F547-86F6-9B4B045F6EEF}" name="2026-05-01" totalsRowFunction="custom" dataDxfId="49" totalsRowDxfId="48">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2026-05-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2026-05-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{3A8C66D0-0121-B94A-963B-D4F350471546}" name="2026-06-01" totalsRowFunction="custom" dataDxfId="74" totalsRowDxfId="6">
+    <tableColumn id="32" xr3:uid="{3A8C66D0-0121-B94A-963B-D4F350471546}" name="2026-06-01" totalsRowFunction="custom" dataDxfId="47" totalsRowDxfId="46">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2026-06-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2026-06-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{8BB2DE1C-C13D-B840-A57E-E8E08A13B45E}" name="2026-07-01" totalsRowFunction="custom" dataDxfId="73" totalsRowDxfId="5">
+    <tableColumn id="33" xr3:uid="{8BB2DE1C-C13D-B840-A57E-E8E08A13B45E}" name="2026-07-01" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="44">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2026-07-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2026-07-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{8DA66CDB-6161-CC4D-A571-DD72FF861D17}" name="2026-08-01" totalsRowFunction="custom" dataDxfId="72" totalsRowDxfId="4">
+    <tableColumn id="34" xr3:uid="{8DA66CDB-6161-CC4D-A571-DD72FF861D17}" name="2026-08-01" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="42">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2026-08-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2026-08-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{4E89C43D-38B3-564B-B587-E203230DA850}" name="2026-09-01" totalsRowFunction="custom" dataDxfId="71" totalsRowDxfId="3">
+    <tableColumn id="35" xr3:uid="{4E89C43D-38B3-564B-B587-E203230DA850}" name="2026-09-01" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="40">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2026-09-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2026-09-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{4DE10C26-4FB6-3F4C-BA3A-36166F4CC466}" name="2026-10-01" totalsRowFunction="custom" dataDxfId="70" totalsRowDxfId="2">
+    <tableColumn id="36" xr3:uid="{4DE10C26-4FB6-3F4C-BA3A-36166F4CC466}" name="2026-10-01" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="38">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2026-10-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2026-10-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{F55F2EEA-2A6C-424C-BBBE-15F2332B5582}" name="2026-11-01" totalsRowFunction="custom" dataDxfId="69" totalsRowDxfId="1">
+    <tableColumn id="37" xr3:uid="{F55F2EEA-2A6C-424C-BBBE-15F2332B5582}" name="2026-11-01" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="36">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2026-11-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2026-11-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{5F503672-BD07-7B4C-BCCD-24CB778A34F6}" name="2026-12-01" totalsRowFunction="custom" dataDxfId="68" totalsRowDxfId="0">
+    <tableColumn id="38" xr3:uid="{5F503672-BD07-7B4C-BCCD-24CB778A34F6}" name="2026-12-01" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="34">
       <totalsRowFormula>SUMIF(Table328[[Movement]:[Movement]],"Credit", Table328[2026-12-01])-SUMIF(Table328[[Movement]:[Movement]],"Debit", Table328[2026-12-01])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -6295,7 +6313,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7525CAA0-1A50-D140-A5F5-D8D57F9F6C72}" name="Table5" displayName="Table5" ref="A1:J4" totalsRowShown="0" headerRowDxfId="67" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7525CAA0-1A50-D140-A5F5-D8D57F9F6C72}" name="Table5" displayName="Table5" ref="A1:J4" totalsRowShown="0" headerRowDxfId="33" tableBorderDxfId="32">
   <autoFilter ref="A1:J4" xr:uid="{7525CAA0-1A50-D140-A5F5-D8D57F9F6C72}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{1CB6D3F1-51C1-684B-93B6-9FA82F9F067F}" name="Movement"/>
@@ -6314,33 +6332,33 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D32C6871-545C-FE44-A877-F290E451E1CF}" name="Table32810" displayName="Table32810" ref="A1:J9" totalsRowCount="1" headerRowDxfId="65" dataDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D32C6871-545C-FE44-A877-F290E451E1CF}" name="Table32810" displayName="Table32810" ref="A1:J9" totalsRowCount="1" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:J8" xr:uid="{92565AF6-51CB-F740-ACD0-AD376C5F8FE0}"/>
   <tableColumns count="10">
-    <tableColumn id="5" xr3:uid="{06CF438D-1451-314D-9C7A-32F80F032CDD}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{D85B60B0-DD6D-9B4D-A4AD-5C8378063533}" name="Account Secondary" totalsRowLabel="Personal Wealth" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="7" xr3:uid="{1DFF1C23-E2EA-B34F-AE16-2538AE6684FC}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="59" totalsRowDxfId="58">
+    <tableColumn id="5" xr3:uid="{06CF438D-1451-314D-9C7A-32F80F032CDD}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{D85B60B0-DD6D-9B4D-A4AD-5C8378063533}" name="Account Secondary" totalsRowLabel="Personal Wealth" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{1DFF1C23-E2EA-B34F-AE16-2538AE6684FC}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="24">
       <totalsRowFormula>SUMIF(Table32810[[Movement]:[Movement]],"Credit", Table32810[2024-05-01])-SUMIF(Table32810[[Movement]:[Movement]],"Debit", Table32810[2024-05-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{907257EB-F7D6-6546-8554-11888A9984A2}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="57" totalsRowDxfId="56">
+    <tableColumn id="8" xr3:uid="{907257EB-F7D6-6546-8554-11888A9984A2}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="22">
       <totalsRowFormula>SUMIF(Table32810[[Movement]:[Movement]],"Credit", Table32810[2024-06-01])-SUMIF(Table32810[[Movement]:[Movement]],"Debit", Table32810[2024-06-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{FE62F661-5418-9F4D-9296-96235170EEE2}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="55" totalsRowDxfId="54">
+    <tableColumn id="9" xr3:uid="{FE62F661-5418-9F4D-9296-96235170EEE2}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="20">
       <totalsRowFormula>SUMIF(Table32810[[Movement]:[Movement]],"Credit", Table32810[2024-07-01])-SUMIF(Table32810[[Movement]:[Movement]],"Debit", Table32810[2024-07-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{EC9FF017-0724-754A-A9F0-748CE63A36A8}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="53" totalsRowDxfId="52">
+    <tableColumn id="10" xr3:uid="{EC9FF017-0724-754A-A9F0-748CE63A36A8}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="18">
       <totalsRowFormula>SUMIF(Table32810[[Movement]:[Movement]],"Credit", Table32810[2024-08-01])-SUMIF(Table32810[[Movement]:[Movement]],"Debit", Table32810[2024-08-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7E66D972-3166-8A43-A093-BCA6C3942C4A}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="51" totalsRowDxfId="50">
+    <tableColumn id="11" xr3:uid="{7E66D972-3166-8A43-A093-BCA6C3942C4A}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="16">
       <totalsRowFormula>SUMIF(Table32810[[Movement]:[Movement]],"Credit", Table32810[2024-09-01])-SUMIF(Table32810[[Movement]:[Movement]],"Debit", Table32810[2024-09-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{840B9A2E-DC2B-9A4F-8617-982B6F6D108A}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="49" totalsRowDxfId="48">
+    <tableColumn id="12" xr3:uid="{840B9A2E-DC2B-9A4F-8617-982B6F6D108A}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="14">
       <totalsRowFormula>SUMIF(Table32810[[Movement]:[Movement]],"Credit", Table32810[2024-10-01])-SUMIF(Table32810[[Movement]:[Movement]],"Debit", Table32810[2024-10-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0D33C5AC-1054-174A-B4A6-9D8972553972}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="47" totalsRowDxfId="46">
+    <tableColumn id="13" xr3:uid="{0D33C5AC-1054-174A-B4A6-9D8972553972}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="12">
       <totalsRowFormula>SUMIF(Table32810[[Movement]:[Movement]],"Credit", Table32810[2024-11-01])-SUMIF(Table32810[[Movement]:[Movement]],"Debit", Table32810[2024-11-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DD93DC27-7299-434C-852A-9DE22656D361}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="44">
+    <tableColumn id="14" xr3:uid="{DD93DC27-7299-434C-852A-9DE22656D361}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
       <totalsRowFormula>SUMIF(Table32810[[Movement]:[Movement]],"Credit", Table32810[2024-12-01])-SUMIF(Table32810[[Movement]:[Movement]],"Debit", Table32810[2024-12-01])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -6665,10 +6683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392F97BE-146F-BF41-B2C2-34275CA1ADBB}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6676,7 +6694,8 @@
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" hidden="1" customWidth="1"/>
     <col min="4" max="5" width="15.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" hidden="1" customWidth="1"/>
+    <col min="7" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -6763,7 +6782,7 @@
         <v>1325</v>
       </c>
       <c r="G3" s="24">
-        <v>1000</v>
+        <v>1325</v>
       </c>
       <c r="H3" s="24">
         <v>1000</v>
@@ -6789,145 +6808,131 @@
         <v>750</v>
       </c>
       <c r="G4" s="24">
-        <v>1000</v>
+        <v>1250</v>
       </c>
       <c r="H4" s="24">
-        <v>1000</v>
+        <v>1250</v>
       </c>
       <c r="I4" s="24">
-        <v>1000</v>
+        <v>1250</v>
       </c>
       <c r="J4" s="24">
-        <v>1000</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="2" customFormat="1" ht="22" x14ac:dyDescent="0.3">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24">
+        <v>5700</v>
+      </c>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+      <c r="A6" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C6" s="24">
         <v>7700</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D6" s="24">
         <v>7700</v>
       </c>
-      <c r="E5" s="56">
+      <c r="E6" s="56">
         <v>7000</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F6" s="24">
         <v>6800</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G6" s="24">
         <v>7000</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H6" s="24">
         <v>7000</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I6" s="24">
         <v>7000</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J6" s="24">
         <v>7000</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="41">
-        <v>500</v>
-      </c>
-      <c r="D6" s="41">
-        <v>1500</v>
-      </c>
-      <c r="E6" s="57">
-        <v>250</v>
-      </c>
-      <c r="F6" s="41">
-        <v>500</v>
-      </c>
-      <c r="G6" s="41">
-        <v>500</v>
-      </c>
-      <c r="H6" s="41">
-        <v>500</v>
-      </c>
-      <c r="I6" s="41">
-        <v>500</v>
-      </c>
-      <c r="J6" s="41">
-        <v>500</v>
-      </c>
-      <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A7" s="40" t="s">
         <v>51</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C7" s="41">
-        <v>8140</v>
+        <v>500</v>
       </c>
       <c r="D7" s="41">
-        <v>8140</v>
-      </c>
-      <c r="E7" s="41">
-        <v>8140</v>
+        <v>1500</v>
+      </c>
+      <c r="E7" s="57">
+        <v>250</v>
       </c>
       <c r="F7" s="41">
-        <v>8140</v>
+        <v>500</v>
       </c>
       <c r="G7" s="41">
-        <v>8140</v>
+        <v>500</v>
       </c>
       <c r="H7" s="41">
-        <v>8140</v>
+        <v>1200</v>
       </c>
       <c r="I7" s="41">
-        <v>8140</v>
+        <v>1000</v>
       </c>
       <c r="J7" s="41">
-        <v>8140</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A8" s="40" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="41">
-        <v>3500</v>
+        <v>8140</v>
       </c>
       <c r="D8" s="41">
-        <v>3578</v>
-      </c>
-      <c r="E8" s="57">
-        <v>3578</v>
+        <v>8140</v>
+      </c>
+      <c r="E8" s="41">
+        <v>8140</v>
       </c>
       <c r="F8" s="41">
-        <v>3578</v>
+        <v>8140</v>
       </c>
       <c r="G8" s="41">
-        <v>3578</v>
+        <v>8140</v>
       </c>
       <c r="H8" s="41">
-        <v>3578</v>
+        <v>8140</v>
       </c>
       <c r="I8" s="41">
-        <v>3578</v>
+        <v>8140</v>
       </c>
       <c r="J8" s="41">
-        <v>3578</v>
+        <v>8140</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -6935,223 +6940,223 @@
         <v>51</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="41">
-        <v>3100</v>
+        <v>3500</v>
       </c>
       <c r="D9" s="41">
-        <v>1700</v>
-      </c>
-      <c r="E9" s="41">
-        <v>1820</v>
+        <v>3578</v>
+      </c>
+      <c r="E9" s="57">
+        <v>3578</v>
       </c>
       <c r="F9" s="41">
-        <v>1820</v>
+        <v>3578</v>
       </c>
       <c r="G9" s="41">
-        <v>0</v>
+        <v>3578</v>
       </c>
       <c r="H9" s="41">
-        <v>0</v>
+        <v>3578</v>
       </c>
       <c r="I9" s="41">
-        <v>0</v>
+        <v>3578</v>
       </c>
       <c r="J9" s="41">
-        <v>0</v>
+        <v>3578</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="39" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A10" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="38">
-        <v>4530</v>
-      </c>
-      <c r="D10" s="38">
-        <v>4530</v>
-      </c>
-      <c r="E10" s="38">
-        <v>4530</v>
-      </c>
-      <c r="F10" s="38">
-        <v>4530</v>
-      </c>
-      <c r="G10" s="38">
-        <v>5600</v>
-      </c>
-      <c r="H10" s="38">
-        <v>4530</v>
-      </c>
-      <c r="I10" s="38">
-        <v>4530</v>
-      </c>
-      <c r="J10" s="38">
-        <v>4530</v>
+      <c r="B10" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="41">
+        <v>3100</v>
+      </c>
+      <c r="D10" s="41">
+        <v>1700</v>
+      </c>
+      <c r="E10" s="41">
+        <v>1820</v>
+      </c>
+      <c r="F10" s="41">
+        <v>1820</v>
+      </c>
+      <c r="G10" s="41">
+        <v>0</v>
+      </c>
+      <c r="H10" s="41">
+        <v>0</v>
+      </c>
+      <c r="I10" s="41">
+        <v>0</v>
+      </c>
+      <c r="J10" s="41">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="39" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A11" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="41">
-        <v>110</v>
-      </c>
-      <c r="D11" s="41">
-        <v>170</v>
-      </c>
-      <c r="E11" s="41">
-        <v>170</v>
-      </c>
-      <c r="F11" s="41">
-        <v>170</v>
-      </c>
-      <c r="G11" s="41">
-        <v>170</v>
-      </c>
-      <c r="H11" s="41">
-        <v>170</v>
-      </c>
-      <c r="I11" s="41">
-        <v>170</v>
-      </c>
-      <c r="J11" s="41">
-        <v>170</v>
+      <c r="B11" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="38">
+        <v>4530</v>
+      </c>
+      <c r="D11" s="38">
+        <v>4530</v>
+      </c>
+      <c r="E11" s="38">
+        <v>4530</v>
+      </c>
+      <c r="F11" s="38">
+        <v>4530</v>
+      </c>
+      <c r="G11" s="38">
+        <v>5600</v>
+      </c>
+      <c r="H11" s="38">
+        <v>5100</v>
+      </c>
+      <c r="I11" s="38">
+        <v>5100</v>
+      </c>
+      <c r="J11" s="38">
+        <v>5100</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="39" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A12" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="38">
-        <v>117</v>
-      </c>
-      <c r="D12" s="38">
-        <v>117</v>
-      </c>
-      <c r="E12" s="38">
-        <v>117</v>
-      </c>
-      <c r="F12" s="38">
-        <v>117</v>
-      </c>
-      <c r="G12" s="38">
-        <v>117</v>
-      </c>
-      <c r="H12" s="38">
-        <v>117</v>
-      </c>
-      <c r="I12" s="38">
-        <v>117</v>
-      </c>
-      <c r="J12" s="38">
-        <v>117</v>
+      <c r="B12" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="41">
+        <v>110</v>
+      </c>
+      <c r="D12" s="41">
+        <v>170</v>
+      </c>
+      <c r="E12" s="41">
+        <v>170</v>
+      </c>
+      <c r="F12" s="41">
+        <v>170</v>
+      </c>
+      <c r="G12" s="41">
+        <v>170</v>
+      </c>
+      <c r="H12" s="41">
+        <v>170</v>
+      </c>
+      <c r="I12" s="41">
+        <v>170</v>
+      </c>
+      <c r="J12" s="41">
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="39" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A13" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="41">
-        <v>1050</v>
-      </c>
-      <c r="D13" s="41">
-        <v>988</v>
-      </c>
-      <c r="E13" s="57">
-        <v>988</v>
-      </c>
-      <c r="F13" s="41">
-        <v>988</v>
-      </c>
-      <c r="G13" s="41">
-        <v>988</v>
-      </c>
-      <c r="H13" s="41">
-        <v>988</v>
-      </c>
-      <c r="I13" s="41">
-        <v>988</v>
-      </c>
-      <c r="J13" s="41">
-        <v>988</v>
+      <c r="B13" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="38">
+        <v>117</v>
+      </c>
+      <c r="D13" s="38">
+        <v>117</v>
+      </c>
+      <c r="E13" s="38">
+        <v>117</v>
+      </c>
+      <c r="F13" s="38">
+        <v>117</v>
+      </c>
+      <c r="G13" s="38">
+        <v>117</v>
+      </c>
+      <c r="H13" s="38">
+        <v>117</v>
+      </c>
+      <c r="I13" s="38">
+        <v>117</v>
+      </c>
+      <c r="J13" s="38">
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="39" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A14" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="38">
-        <v>1200</v>
-      </c>
-      <c r="D14" s="38">
-        <v>560</v>
-      </c>
-      <c r="E14" s="38">
-        <v>560</v>
-      </c>
-      <c r="F14" s="38">
-        <v>560</v>
-      </c>
-      <c r="G14" s="38">
-        <v>560</v>
-      </c>
-      <c r="H14" s="38">
-        <v>560</v>
-      </c>
-      <c r="I14" s="38">
-        <v>560</v>
-      </c>
-      <c r="J14" s="38">
-        <v>560</v>
+      <c r="B14" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="41">
+        <v>1050</v>
+      </c>
+      <c r="D14" s="41">
+        <v>988</v>
+      </c>
+      <c r="E14" s="57">
+        <v>988</v>
+      </c>
+      <c r="F14" s="41">
+        <v>988</v>
+      </c>
+      <c r="G14" s="41">
+        <v>988</v>
+      </c>
+      <c r="H14" s="41">
+        <v>988</v>
+      </c>
+      <c r="I14" s="41">
+        <v>988</v>
+      </c>
+      <c r="J14" s="41">
+        <v>988</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="39" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A15" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="41">
-        <v>440</v>
-      </c>
-      <c r="D15" s="41">
-        <v>440</v>
-      </c>
-      <c r="E15" s="41">
-        <v>440</v>
-      </c>
-      <c r="F15" s="41">
-        <v>440</v>
-      </c>
-      <c r="G15" s="41">
-        <v>440</v>
-      </c>
-      <c r="H15" s="41">
-        <v>440</v>
-      </c>
-      <c r="I15" s="41">
-        <v>440</v>
-      </c>
-      <c r="J15" s="41">
-        <v>440</v>
+      <c r="B15" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="38">
+        <v>1200</v>
+      </c>
+      <c r="D15" s="38">
+        <v>560</v>
+      </c>
+      <c r="E15" s="38">
+        <v>560</v>
+      </c>
+      <c r="F15" s="38">
+        <v>560</v>
+      </c>
+      <c r="G15" s="38">
+        <v>560</v>
+      </c>
+      <c r="H15" s="38">
+        <v>560</v>
+      </c>
+      <c r="I15" s="38">
+        <v>610</v>
+      </c>
+      <c r="J15" s="38">
+        <v>610</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="39" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -7159,159 +7164,159 @@
         <v>51</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C16" s="41">
-        <v>600</v>
+        <v>440</v>
       </c>
       <c r="D16" s="41">
-        <v>600</v>
+        <v>440</v>
       </c>
       <c r="E16" s="41">
-        <v>0</v>
+        <v>440</v>
       </c>
       <c r="F16" s="41">
-        <v>0</v>
+        <v>440</v>
       </c>
       <c r="G16" s="41">
-        <v>0</v>
+        <v>440</v>
       </c>
       <c r="H16" s="41">
-        <v>0</v>
+        <v>440</v>
       </c>
       <c r="I16" s="41">
-        <v>0</v>
+        <v>440</v>
       </c>
       <c r="J16" s="41">
-        <v>0</v>
+        <v>440</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="39" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A17" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="38">
-        <v>3500</v>
-      </c>
-      <c r="D17" s="38">
-        <v>3500</v>
-      </c>
-      <c r="E17" s="58">
-        <v>3500</v>
-      </c>
-      <c r="F17" s="38">
-        <v>3500</v>
-      </c>
-      <c r="G17" s="38">
-        <v>3500</v>
-      </c>
-      <c r="H17" s="38">
-        <v>3500</v>
-      </c>
-      <c r="I17" s="38">
-        <v>3500</v>
-      </c>
-      <c r="J17" s="38">
-        <v>3500</v>
+      <c r="B17" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="41">
+        <v>600</v>
+      </c>
+      <c r="D17" s="41">
+        <v>600</v>
+      </c>
+      <c r="E17" s="41">
+        <v>0</v>
+      </c>
+      <c r="F17" s="41">
+        <v>0</v>
+      </c>
+      <c r="G17" s="41">
+        <v>0</v>
+      </c>
+      <c r="H17" s="41">
+        <v>0</v>
+      </c>
+      <c r="I17" s="41">
+        <v>0</v>
+      </c>
+      <c r="J17" s="41">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="39" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A18" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="41">
-        <v>1000</v>
-      </c>
-      <c r="D18" s="41">
-        <v>1000</v>
-      </c>
-      <c r="E18" s="57">
-        <v>1000</v>
-      </c>
-      <c r="F18" s="41">
-        <v>1000</v>
-      </c>
-      <c r="G18" s="41">
-        <v>1000</v>
-      </c>
-      <c r="H18" s="41">
-        <v>1000</v>
-      </c>
-      <c r="I18" s="41">
-        <v>1000</v>
-      </c>
-      <c r="J18" s="41">
-        <v>1000</v>
+      <c r="B18" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="38">
+        <v>3500</v>
+      </c>
+      <c r="D18" s="38">
+        <v>3500</v>
+      </c>
+      <c r="E18" s="58">
+        <v>3500</v>
+      </c>
+      <c r="F18" s="38">
+        <v>3500</v>
+      </c>
+      <c r="G18" s="38">
+        <v>3500</v>
+      </c>
+      <c r="H18" s="38">
+        <v>4500</v>
+      </c>
+      <c r="I18" s="38">
+        <v>4000</v>
+      </c>
+      <c r="J18" s="38">
+        <v>4000</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="39" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A19" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="38">
+      <c r="B19" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="41">
         <v>1000</v>
       </c>
-      <c r="D19" s="38">
-        <v>1500</v>
-      </c>
-      <c r="E19" s="58">
-        <v>250</v>
-      </c>
-      <c r="F19" s="38">
-        <v>500</v>
-      </c>
-      <c r="G19" s="38">
-        <v>900</v>
-      </c>
-      <c r="H19" s="38">
-        <v>500</v>
-      </c>
-      <c r="I19" s="38">
-        <v>500</v>
-      </c>
-      <c r="J19" s="38">
-        <v>500</v>
+      <c r="D19" s="41">
+        <v>1000</v>
+      </c>
+      <c r="E19" s="57">
+        <v>1000</v>
+      </c>
+      <c r="F19" s="41">
+        <v>1000</v>
+      </c>
+      <c r="G19" s="41">
+        <v>1000</v>
+      </c>
+      <c r="H19" s="41">
+        <v>1000</v>
+      </c>
+      <c r="I19" s="41">
+        <v>1000</v>
+      </c>
+      <c r="J19" s="41">
+        <v>1000</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="39" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A20" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="41">
-        <v>5000</v>
-      </c>
-      <c r="D20" s="41">
-        <v>4300</v>
-      </c>
-      <c r="E20" s="41">
-        <v>3000</v>
-      </c>
-      <c r="F20" s="41">
-        <v>3500</v>
-      </c>
-      <c r="G20" s="41">
-        <v>3200</v>
-      </c>
-      <c r="H20" s="41">
-        <v>3800</v>
-      </c>
-      <c r="I20" s="41">
-        <v>3800</v>
-      </c>
-      <c r="J20" s="41">
-        <v>3800</v>
+      <c r="B20" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="38">
+        <v>1000</v>
+      </c>
+      <c r="D20" s="38">
+        <v>1500</v>
+      </c>
+      <c r="E20" s="58">
+        <v>250</v>
+      </c>
+      <c r="F20" s="38">
+        <v>500</v>
+      </c>
+      <c r="G20" s="38">
+        <v>900</v>
+      </c>
+      <c r="H20" s="38">
+        <v>300</v>
+      </c>
+      <c r="I20" s="38">
+        <v>300</v>
+      </c>
+      <c r="J20" s="38">
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="39" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -7319,47 +7324,49 @@
         <v>51</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="C21" s="41">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="D21" s="41">
-        <v>0</v>
+        <v>4300</v>
       </c>
       <c r="E21" s="41">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="F21" s="41">
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="G21" s="41">
-        <v>0</v>
+        <v>3200</v>
       </c>
       <c r="H21" s="41">
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="I21" s="41">
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="J21" s="41">
-        <v>0</v>
+        <v>3500</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" s="39" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A22" s="40" t="s">
         <v>51</v>
       </c>
       <c r="B22" s="40" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C22" s="41">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="D22" s="41">
-        <v>200</v>
-      </c>
-      <c r="E22" s="41"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="41">
+        <v>0</v>
+      </c>
       <c r="F22" s="41">
         <v>0</v>
       </c>
@@ -7380,30 +7387,30 @@
       <c r="A23" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="38">
-        <v>1000</v>
-      </c>
-      <c r="D23" s="38">
-        <v>1000</v>
-      </c>
-      <c r="E23" s="38">
+      <c r="B23" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="41">
+        <v>500</v>
+      </c>
+      <c r="D23" s="41">
+        <v>200</v>
+      </c>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41">
         <v>0</v>
       </c>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38">
-        <v>500</v>
-      </c>
-      <c r="H23" s="38">
-        <v>1000</v>
-      </c>
-      <c r="I23" s="38">
-        <v>1000</v>
-      </c>
-      <c r="J23" s="38">
-        <v>1000</v>
+      <c r="G23" s="41">
+        <v>0</v>
+      </c>
+      <c r="H23" s="41">
+        <v>0</v>
+      </c>
+      <c r="I23" s="41">
+        <v>0</v>
+      </c>
+      <c r="J23" s="41">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -7411,31 +7418,29 @@
         <v>51</v>
       </c>
       <c r="B24" s="42" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C24" s="38">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="D24" s="38">
-        <v>200</v>
-      </c>
-      <c r="E24" s="58">
-        <v>200</v>
-      </c>
-      <c r="F24" s="38">
-        <v>200</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="E24" s="38">
+        <v>0</v>
+      </c>
+      <c r="F24" s="38"/>
       <c r="G24" s="38">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="H24" s="38">
-        <v>200</v>
+        <v>750</v>
       </c>
       <c r="I24" s="38">
-        <v>200</v>
+        <v>750</v>
       </c>
       <c r="J24" s="38">
-        <v>200</v>
+        <v>750</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -7443,58 +7448,62 @@
         <v>51</v>
       </c>
       <c r="B25" s="42" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="C25" s="38">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D25" s="38">
-        <v>0</v>
-      </c>
-      <c r="E25" s="38">
-        <v>0</v>
+        <v>200</v>
+      </c>
+      <c r="E25" s="58">
+        <v>200</v>
       </c>
       <c r="F25" s="38">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="G25" s="38">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="H25" s="38">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="I25" s="38">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="J25" s="38">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="57">
-        <v>640</v>
-      </c>
-      <c r="F26" s="41">
+      <c r="B26" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="38">
         <v>0</v>
       </c>
-      <c r="G26" s="41">
+      <c r="D26" s="38">
         <v>0</v>
       </c>
-      <c r="H26" s="41">
+      <c r="E26" s="38">
         <v>0</v>
       </c>
-      <c r="I26" s="41">
+      <c r="F26" s="38">
         <v>0</v>
       </c>
-      <c r="J26" s="41">
+      <c r="G26" s="38">
+        <v>0</v>
+      </c>
+      <c r="H26" s="38">
+        <v>0</v>
+      </c>
+      <c r="I26" s="38">
+        <v>0</v>
+      </c>
+      <c r="J26" s="38">
         <v>0</v>
       </c>
     </row>
@@ -7503,33 +7512,43 @@
         <v>51</v>
       </c>
       <c r="B27" s="43" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C27" s="41"/>
       <c r="D27" s="41"/>
-      <c r="E27" s="41">
-        <v>600</v>
+      <c r="E27" s="57">
+        <v>640</v>
       </c>
       <c r="F27" s="41">
-        <v>600</v>
-      </c>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="41"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="41">
+        <v>0</v>
+      </c>
+      <c r="H27" s="41">
+        <v>0</v>
+      </c>
+      <c r="I27" s="41">
+        <v>0</v>
+      </c>
+      <c r="J27" s="41">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:10" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A28" s="43" t="s">
         <v>51</v>
       </c>
       <c r="B28" s="43" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C28" s="41"/>
       <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
+      <c r="E28" s="41">
+        <v>600</v>
+      </c>
       <c r="F28" s="41">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="G28" s="41"/>
       <c r="H28" s="41"/>
@@ -7537,71 +7556,109 @@
       <c r="J28" s="41"/>
     </row>
     <row r="29" spans="1:10" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41">
+        <v>500</v>
+      </c>
+      <c r="G29" s="41">
+        <v>500</v>
+      </c>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="41"/>
+    </row>
+    <row r="30" spans="1:10" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+      <c r="A30" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41">
+        <v>1000</v>
+      </c>
+      <c r="I30" s="41"/>
+      <c r="J30" s="41"/>
+    </row>
+    <row r="31" spans="1:10" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+      <c r="A31" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="41">
+      <c r="C31" s="41">
         <v>0</v>
       </c>
-      <c r="D29" s="41">
+      <c r="D31" s="41">
         <v>500</v>
       </c>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41">
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="59">
         <v>1000</v>
       </c>
-      <c r="H29" s="41">
-        <v>1000</v>
-      </c>
-      <c r="I29" s="41">
-        <v>1000</v>
-      </c>
-      <c r="J29" s="41">
-        <v>1000</v>
+      <c r="H31" s="41">
+        <v>5000</v>
+      </c>
+      <c r="I31" s="41">
+        <v>500</v>
+      </c>
+      <c r="J31" s="41">
+        <v>500</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A30" s="33" t="s">
+    <row r="32" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="A32" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="B30" s="33" t="s">
+      <c r="B32" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C32" s="13">
         <f>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-05-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-05-01]])</f>
         <v>538</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D32" s="13">
         <f>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-06-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-06-01]])</f>
         <v>1502</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E32" s="13">
         <f>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-07-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-07-01]])</f>
         <v>142</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F32" s="13">
         <f>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-08-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-08-01]])</f>
         <v>-168</v>
       </c>
-      <c r="G30" s="13">
+      <c r="G32" s="13">
         <f>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-09-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-09-01]])</f>
-        <v>207</v>
-      </c>
-      <c r="H30" s="13">
+        <v>282</v>
+      </c>
+      <c r="H32" s="13">
         <f>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-10-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-10-01]])</f>
-        <v>577</v>
-      </c>
-      <c r="I30" s="13">
+        <v>7</v>
+      </c>
+      <c r="I32" s="13">
         <f>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-11-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-11-01]])</f>
-        <v>577</v>
-      </c>
-      <c r="J30" s="13">
+        <v>457</v>
+      </c>
+      <c r="J32" s="13">
         <f>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-12-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-12-01]])</f>
-        <v>577</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -7618,7 +7675,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7626,8 +7683,8 @@
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="35.33203125" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" hidden="1" customWidth="1"/>
-    <col min="6" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.1640625" hidden="1" customWidth="1"/>
+    <col min="7" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -7968,10 +8025,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FCEDF0D-72A7-F24E-9B15-0D8218302531}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7980,7 +8037,8 @@
     <col min="2" max="2" width="35.33203125" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.1640625" hidden="1" customWidth="1"/>
+    <col min="7" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -8080,75 +8138,99 @@
       </c>
     </row>
     <row r="4" spans="1:10" s="4" customFormat="1" ht="22" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19">
+        <v>110</v>
+      </c>
+      <c r="H4" s="19">
+        <v>110</v>
+      </c>
+      <c r="I4" s="19">
+        <v>110</v>
+      </c>
+      <c r="J4" s="19">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="4" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C5" s="12">
         <v>0</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D5" s="12">
         <v>230</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E5" s="12">
         <v>230</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F5" s="12">
         <v>230</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G5" s="12">
         <v>230</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H5" s="12">
         <v>230</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I5" s="12">
         <v>230</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J5" s="12">
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+    <row r="6" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B6" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C6" s="13">
         <f>SUMIF(Table323[[Movement]:[Movement]],"Credit", Table323[2024-05-01])-SUMIF(Table323[[Movement]:[Movement]],"Debit", Table323[2024-05-01])</f>
         <v>500</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D6" s="13">
         <f>SUMIF(Table323[[Movement]:[Movement]],"Credit", Table323[2024-06-01])-SUMIF(Table323[[Movement]:[Movement]],"Debit", Table323[2024-06-01])</f>
         <v>1070</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E6" s="13">
         <f>SUMIF(Table323[[Movement]:[Movement]],"Credit", Table323[2024-07-01])-SUMIF(Table323[[Movement]:[Movement]],"Debit", Table323[2024-07-01])</f>
         <v>-180</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F6" s="13">
         <f>SUMIF(Table323[[Movement]:[Movement]],"Credit", Table323[2024-08-01])-SUMIF(Table323[[Movement]:[Movement]],"Debit", Table323[2024-08-01])</f>
         <v>70</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G6" s="13">
         <f>SUMIF(Table323[[Movement]:[Movement]],"Credit", Table323[2024-09-01])-SUMIF(Table323[[Movement]:[Movement]],"Debit", Table323[2024-09-01])</f>
-        <v>70</v>
-      </c>
-      <c r="H5" s="13">
+        <v>-40</v>
+      </c>
+      <c r="H6" s="13">
         <f>SUMIF(Table323[[Movement]:[Movement]],"Credit", Table323[2024-10-01])-SUMIF(Table323[[Movement]:[Movement]],"Debit", Table323[2024-10-01])</f>
-        <v>70</v>
-      </c>
-      <c r="I5" s="13">
+        <v>-40</v>
+      </c>
+      <c r="I6" s="13">
         <f>SUMIF(Table323[[Movement]:[Movement]],"Credit", Table323[2024-11-01])-SUMIF(Table323[[Movement]:[Movement]],"Debit", Table323[2024-11-01])</f>
-        <v>70</v>
-      </c>
-      <c r="J5" s="13">
+        <v>-40</v>
+      </c>
+      <c r="J6" s="13">
         <f>SUMIF(Table323[[Movement]:[Movement]],"Credit", Table323[2024-12-01])-SUMIF(Table323[[Movement]:[Movement]],"Debit", Table323[2024-12-01])</f>
-        <v>70</v>
+        <v>-40</v>
       </c>
     </row>
   </sheetData>
@@ -8747,7 +8829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2656F070-2FBF-4D4F-8695-FA36A20F8B06}">
   <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding latest source files
</commit_message>
<xml_diff>
--- a/source files/budget_jeanre.xlsx
+++ b/source files/budget_jeanre.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/GIT Repos/ftrack/source files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/GIT-Repos/ftrack/source files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14543A7-9672-D248-9DDD-0B2EC1176951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98F514B-3EA1-6F4A-9F27-A4254BC174C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-107200" yWindow="-1100" windowWidth="38400" windowHeight="23500" xr2:uid="{F25DD163-696E-F842-A897-5E899A2812A7}"/>
+    <workbookView xWindow="-48660" yWindow="-5900" windowWidth="48660" windowHeight="28300" xr2:uid="{F25DD163-696E-F842-A897-5E899A2812A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Jeanre Transactional" sheetId="11" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="93">
   <si>
     <t>Jeanre Transactional</t>
   </si>
@@ -317,6 +317,12 @@
   <si>
     <t>Retained Balance</t>
   </si>
+  <si>
+    <t>Accounts</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
 </sst>
 </file>
 
@@ -325,7 +331,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -470,6 +476,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -655,7 +668,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -720,6 +733,7 @@
     <xf numFmtId="44" fontId="20" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="11" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="21" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6032,8 +6046,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3E63981-326C-D143-B66A-6C003C4E74A8}" name="Table32" displayName="Table32" ref="A1:J33" totalsRowCount="1" headerRowDxfId="221" dataDxfId="220">
-  <autoFilter ref="A1:J32" xr:uid="{92565AF6-51CB-F740-ACD0-AD376C5F8FE0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3E63981-326C-D143-B66A-6C003C4E74A8}" name="Table32" displayName="Table32" ref="A1:J35" totalsRowCount="1" headerRowDxfId="221" dataDxfId="220">
+  <autoFilter ref="A1:J34" xr:uid="{92565AF6-51CB-F740-ACD0-AD376C5F8FE0}"/>
   <tableColumns count="10">
     <tableColumn id="5" xr3:uid="{8651B483-0F4C-9745-8034-DD83AE8DA141}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="219" totalsRowDxfId="9"/>
     <tableColumn id="6" xr3:uid="{2F7AE88F-4B40-4240-BF3E-94BC56EB2208}" name="Account Secondary" totalsRowLabel="Jeanre Transactional" dataDxfId="218" totalsRowDxfId="8"/>
@@ -6708,10 +6722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392F97BE-146F-BF41-B2C2-34275CA1ADBB}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="163" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6719,8 +6733,8 @@
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" hidden="1" customWidth="1"/>
     <col min="4" max="5" width="15.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="15.1640625" hidden="1" customWidth="1"/>
-    <col min="8" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="15.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -6837,10 +6851,10 @@
       </c>
       <c r="H4" s="24"/>
       <c r="I4" s="24">
-        <v>1250</v>
+        <v>250</v>
       </c>
       <c r="J4" s="24">
-        <v>1250</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="2" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -6858,8 +6872,12 @@
       <c r="H5" s="24">
         <v>0</v>
       </c>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
+      <c r="I5" s="24">
+        <v>3500</v>
+      </c>
+      <c r="J5" s="24">
+        <v>800</v>
+      </c>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A6" s="55" t="s">
@@ -6905,10 +6923,10 @@
         <v>7300</v>
       </c>
       <c r="I7" s="24">
-        <v>7000</v>
+        <v>7750</v>
       </c>
       <c r="J7" s="24">
-        <v>7000</v>
+        <v>7750</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -6937,10 +6955,10 @@
         <v>1000</v>
       </c>
       <c r="I8" s="41">
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="J8" s="41">
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="K8" s="7"/>
     </row>
@@ -7354,10 +7372,10 @@
         <v>200</v>
       </c>
       <c r="I21" s="38">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="J21" s="38">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="39" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -7389,7 +7407,7 @@
         <v>3500</v>
       </c>
       <c r="J22" s="41">
-        <v>3500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="39" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -7478,10 +7496,10 @@
         <v>1000</v>
       </c>
       <c r="I25" s="38">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="J25" s="38">
-        <v>750</v>
+        <v>500</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -7603,19 +7621,17 @@
         <v>51</v>
       </c>
       <c r="B30" s="43" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C30" s="41"/>
       <c r="D30" s="41"/>
       <c r="E30" s="41"/>
-      <c r="F30" s="41">
-        <v>500</v>
-      </c>
-      <c r="G30" s="41">
-        <v>500</v>
-      </c>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
       <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
+      <c r="I30" s="64">
+        <v>2227</v>
+      </c>
       <c r="J30" s="41"/>
     </row>
     <row r="31" spans="1:10" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -7623,7 +7639,7 @@
         <v>51</v>
       </c>
       <c r="B31" s="43" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C31" s="41"/>
       <c r="D31" s="41"/>
@@ -7631,73 +7647,111 @@
       <c r="F31" s="41"/>
       <c r="G31" s="41"/>
       <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
+      <c r="I31" s="41">
+        <v>2065</v>
+      </c>
+      <c r="J31" s="41">
+        <v>1350</v>
+      </c>
     </row>
     <row r="32" spans="1:10" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41">
+        <v>500</v>
+      </c>
+      <c r="G32" s="41">
+        <v>500</v>
+      </c>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+    </row>
+    <row r="33" spans="1:10" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+      <c r="A33" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="41"/>
+    </row>
+    <row r="34" spans="1:10" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+      <c r="A34" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="41">
+      <c r="C34" s="41">
         <v>0</v>
       </c>
-      <c r="D32" s="41">
+      <c r="D34" s="41">
         <v>500</v>
       </c>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="59">
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="59">
         <v>5000</v>
       </c>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41">
+      <c r="H34" s="41"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="41">
         <v>500</v>
       </c>
-      <c r="J32" s="41">
-        <v>500</v>
-      </c>
     </row>
-    <row r="33" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A33" s="33" t="s">
+    <row r="35" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="A35" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B35" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C35" s="13">
         <f>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-05-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-05-01]])</f>
         <v>538</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D35" s="13">
         <f>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-06-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-06-01]])</f>
         <v>1502</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E35" s="13">
         <f>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-07-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-07-01]])</f>
         <v>142</v>
       </c>
-      <c r="F33" s="13">
+      <c r="F35" s="13">
         <f>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-08-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-08-01]])</f>
         <v>-168</v>
       </c>
-      <c r="G33" s="13">
+      <c r="G35" s="13">
         <f>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-09-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-09-01]])</f>
         <v>1982</v>
       </c>
-      <c r="H33" s="13">
+      <c r="H35" s="13">
         <f>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-10-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-10-01]])</f>
         <v>-473</v>
       </c>
-      <c r="I33" s="13">
+      <c r="I35" s="13">
         <f>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-11-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-11-01]])</f>
-        <v>-43</v>
-      </c>
-      <c r="J33" s="13">
+        <v>65</v>
+      </c>
+      <c r="J35" s="13">
         <f>SUMIF(Table32[[#Data],[#Totals],[Movement]],"Credit", Table32[[#Data],[#Totals],[2024-12-01]])-SUMIF(Table32[[#Data],[#Totals],[Movement]],"Debit", Table32[[#Data],[#Totals],[2024-12-01]])</f>
-        <v>-43</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -7713,8 +7767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3966FA5A-65C3-DE4D-964E-13540A60950B}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7722,8 +7776,8 @@
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="35.33203125" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="7" width="15.1640625" hidden="1" customWidth="1"/>
-    <col min="8" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="15.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -7816,10 +7870,10 @@
         <v>500</v>
       </c>
       <c r="I3" s="41">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="J3" s="41">
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -7848,10 +7902,10 @@
         <v>7300</v>
       </c>
       <c r="I4" s="38">
-        <v>7000</v>
+        <v>7750</v>
       </c>
       <c r="J4" s="38">
-        <v>7000</v>
+        <v>7750</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="39" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -8057,11 +8111,11 @@
       </c>
       <c r="I11" s="47">
         <f>SUMIF(Table325[[Movement]:[Movement]],"Credit", Table325[2024-11-01])-SUMIF(Table325[[Movement]:[Movement]],"Debit",Table325[2024-11-01])</f>
-        <v>990</v>
+        <v>40</v>
       </c>
       <c r="J11" s="47">
         <f>SUMIF(Table325[[Movement]:[Movement]],"Credit", Table325[2024-12-01])-SUMIF(Table325[[Movement]:[Movement]],"Debit",Table325[2024-12-01])</f>
-        <v>990</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>